<commit_message>
Finished writing implementation of the RESTDispatch classes
</commit_message>
<xml_diff>
--- a/doc/systems/Beaglebone REST.xlsx
+++ b/doc/systems/Beaglebone REST.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="76">
   <si>
     <t>Notes</t>
   </si>
@@ -84,9 +84,6 @@
     <t>waypointStrengthMax</t>
   </si>
   <si>
-    <t>offshore</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>See Arduino REST documentation for details</t>
+  </si>
+  <si>
+    <t>autonomous</t>
   </si>
 </sst>
 </file>
@@ -386,6 +386,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,15 +403,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -701,44 +701,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -768,10 +768,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -785,10 +785,10 @@
         <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -802,10 +802,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,10 +819,10 @@
         <v>15</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -836,10 +836,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -853,10 +853,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,10 +870,10 @@
         <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -887,10 +887,10 @@
         <v>18</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,80 +904,80 @@
         <v>18</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -986,64 +986,64 @@
         <v>15</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>14</v>
@@ -1053,123 +1053,123 @@
         <v>15</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>14</v>
@@ -1179,10 +1179,10 @@
         <v>15</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -1195,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1210,13 +1210,13 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1231,10 +1231,10 @@
         <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1249,15 +1249,15 @@
         <v>15</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1265,40 +1265,40 @@
         <v>3</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Clarified some details of the REST interface
</commit_message>
<xml_diff>
--- a/doc/systems/Beaglebone REST.xlsx
+++ b/doc/systems/Beaglebone REST.xlsx
@@ -15,11 +15,12 @@
     <sheet name="REST" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
   <si>
     <t>Notes</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Resets the Arduino</t>
   </si>
   <si>
-    <t xml:space="preserve">The URL request shall be of the form http{s}://&lt;host&gt;/&lt;top level&gt;/&lt;second level&gt;/&lt;third level&gt;/. GET requests shall return the value of the item requested as a JSON object. In order to write an item, the user shall make a POST request with a JSON object containing the data to be written. </t>
-  </si>
-  <si>
     <t>Behavior Note</t>
   </si>
   <si>
@@ -247,6 +245,9 @@
   </si>
   <si>
     <t>autonomous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The URL request shall be of the form http{s}://&lt;host&gt;/&lt;top level&gt;/&lt;second level&gt;/&lt;third level&gt;/. GET requests shall return the value of the item requested as a JSON object. In order to write an item, the user shall make a POST request with a JSON object containing the data to be written. The JSON object must contain a key-value pair with the key value equal to the second level name. All other keys shall be ignored. If the expected key is not present, return the current value. The only exception is the various waypoint writing commands, which expect a complete waypoint object. </t>
   </si>
 </sst>
 </file>
@@ -686,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -702,7 +703,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -710,9 +711,9 @@
       <c r="E1" s="13"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:6" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -722,7 +723,7 @@
     </row>
     <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -732,7 +733,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -839,7 +840,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -856,7 +857,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -873,7 +874,7 @@
         <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -890,7 +891,7 @@
         <v>36</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,7 +908,7 @@
         <v>36</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -915,7 +916,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
@@ -924,7 +925,7 @@
         <v>36</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -938,7 +939,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -955,7 +956,7 @@
         <v>35</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -972,7 +973,7 @@
         <v>35</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -989,7 +990,7 @@
         <v>35</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1003,7 +1004,7 @@
         <v>35</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1020,7 +1021,7 @@
         <v>36</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1038,7 +1039,7 @@
         <v>35</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1056,7 +1057,7 @@
         <v>35</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -1074,7 +1075,7 @@
         <v>36</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1094,7 +1095,7 @@
         <v>36</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1112,7 +1113,7 @@
         <v>36</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -1128,7 +1129,7 @@
         <v>35</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1146,7 +1147,7 @@
         <v>35</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1164,7 +1165,7 @@
         <v>35</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1182,7 +1183,7 @@
         <v>35</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -1198,7 +1199,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1216,7 +1217,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1234,7 +1235,7 @@
         <v>35</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1252,7 +1253,7 @@
         <v>35</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
@@ -1273,7 +1274,7 @@
     </row>
     <row r="36" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1282,15 +1283,15 @@
         <v>35</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
@@ -1298,7 +1299,7 @@
         <v>35</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>